<commit_message>
Update flow split to correct Upper Basin pre 1922 water rights
In Model Guide
In R Code
In Pre 1922 folder
</commit_message>
<xml_diff>
--- a/Pre1922CompactWaterUse/PrePostCompactWaterRights.xlsx
+++ b/Pre1922CompactWaterUse/PrePostCompactWaterRights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20380"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\PreCompact\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\Pre1922CompactWaterUse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23362F1-3372-4832-9107-BB16F7962DF6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA102D6B-917A-4E67-8955-187F4370D53A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6350" xr2:uid="{103A74F2-4913-4D84-B9FD-026CB70CED0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6345" xr2:uid="{103A74F2-4913-4D84-B9FD-026CB70CED0B}"/>
   </bookViews>
   <sheets>
     <sheet name="FromSheet" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
   <si>
     <t>State</t>
   </si>
@@ -205,7 +205,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -522,97 +522,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58A434C0-4C67-4213-99E0-4DA4B9ACBBE5}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" customWidth="1"/>
-    <col min="3" max="3" width="35.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="4">
         <v>0.53849999999999998</v>
       </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C4" s="4">
+        <f>D4-B4</f>
+        <v>0.4415</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="4">
         <v>0.54743299999999995</v>
       </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="D5" s="4">
+        <f>SUM(B5,C5)</f>
+        <v>0.59743299999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="5">
         <v>1.1100000000000001</v>
       </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="4">
+        <f>D6-B6</f>
+        <v>1.39</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="4">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="4">
+        <f>D7-B7</f>
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.41499999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="12">
         <v>1.2500000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="4">
+        <f>0.3-B8</f>
+        <v>0.28749999999999998</v>
+      </c>
+      <c r="D8" s="4">
+        <f>SUM(B8:C8)</f>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B9" s="4">
         <v>1.5029999999999999</v>
       </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="4">
+        <f>2.8-B9</f>
+        <v>1.2969999999999999</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" ref="D9:D10" si="0">SUM(B9:C9)</f>
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="4">
         <v>2.0150000000000001</v>
       </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="4">
+        <f>4.4-B10</f>
+        <v>2.3850000000000002</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>20</v>
       </c>
@@ -620,9 +669,16 @@
         <f>SUM(B4:B7)</f>
         <v>2.2639330000000002</v>
       </c>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="9">
+        <f>SUM(C4:C7)</f>
+        <v>2.2284999999999999</v>
+      </c>
+      <c r="D11" s="9">
+        <f>SUM(D4:D7)</f>
+        <v>4.4924330000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>21</v>
       </c>
@@ -630,14 +686,21 @@
         <f>SUM(B8:B10)</f>
         <v>3.5305</v>
       </c>
-      <c r="C12" s="8"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="9">
+        <f t="shared" ref="C12:D12" si="1">SUM(C8:C10)</f>
+        <v>3.9695</v>
+      </c>
+      <c r="D12" s="9">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -652,21 +715,21 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:A27"/>
+      <selection activeCell="C3" sqref="C3:D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="35.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>0</v>
       </c>
@@ -683,7 +746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -701,7 +764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -719,7 +782,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -737,7 +800,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -755,7 +818,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
@@ -773,15 +836,15 @@
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -799,18 +862,18 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" customWidth="1"/>
-    <col min="5" max="5" width="35.1796875" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -827,7 +890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -845,7 +908,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -863,7 +926,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -881,7 +944,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -894,7 +957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
@@ -912,17 +975,17 @@
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>16</v>
       </c>

</xml_diff>